<commit_message>
3 ml for more viscous solutions
</commit_message>
<xml_diff>
--- a/Viscosity/solutionsNrheology.xlsx
+++ b/Viscosity/solutionsNrheology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oskat\OneDrive - Instituto Tecnologico y de Estudios Superiores de Monterrey\Documents\MNT_ITESM_Thesis\Viscosity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE73342-2F70-4C8E-8A68-FC28BE25D076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFE4243-8B2F-4758-BF94-D359C234F316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="5490" windowWidth="15345" windowHeight="11385" activeTab="2" xr2:uid="{B7136CE4-8007-46B5-82B9-4587FFE551E7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="106">
   <si>
     <t>Pa.s</t>
   </si>
@@ -482,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -622,6 +622,9 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1614,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369913E4-9BA3-456A-A7BC-B2736832302E}">
-  <dimension ref="A1:L127"/>
+  <dimension ref="A1:L132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,6 +1647,11 @@
       </c>
       <c r="I1" s="32"/>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="4">
+        <v>3000</v>
+      </c>
+    </row>
     <row r="3" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>97</v>
@@ -1917,16 +1925,16 @@
         <v>20</v>
       </c>
       <c r="D14" s="20">
-        <f>$D$21*((100-C14)/100)</f>
-        <v>1420.8000000000002</v>
+        <f>$D$22*((100-C14)/100)</f>
+        <v>2131.2000000000003</v>
       </c>
       <c r="E14" s="20">
         <f>D14/$D$20</f>
-        <v>1600.0000000000002</v>
+        <v>2400.0000000000005</v>
       </c>
       <c r="F14" s="20">
-        <f>$D$21*(C14/100)</f>
-        <v>355.20000000000005</v>
+        <f>$D$22*(C14/100)</f>
+        <v>532.80000000000007</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -1938,16 +1946,16 @@
         <v>25</v>
       </c>
       <c r="D15" s="20">
-        <f>$D$21*((100-C15)/100)</f>
-        <v>1332</v>
+        <f t="shared" ref="D15:D18" si="1">$D$22*((100-C15)/100)</f>
+        <v>1998</v>
       </c>
       <c r="E15" s="20">
         <f>D15/$D$20</f>
-        <v>1500</v>
+        <v>2250</v>
       </c>
       <c r="F15" s="20">
-        <f>$D$21*(C15/100)</f>
-        <v>444</v>
+        <f t="shared" ref="F15:F18" si="2">$D$22*(C15/100)</f>
+        <v>666</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -1959,16 +1967,16 @@
         <v>30</v>
       </c>
       <c r="D16" s="20">
-        <f>$D$21*((100-C16)/100)</f>
-        <v>1243.1999999999998</v>
+        <f t="shared" si="1"/>
+        <v>1864.8</v>
       </c>
       <c r="E16" s="20">
         <f>D16/$D$20</f>
-        <v>1399.9999999999998</v>
+        <v>2100</v>
       </c>
       <c r="F16" s="20">
-        <f>$D$21*(C16/100)</f>
-        <v>532.79999999999995</v>
+        <f t="shared" si="2"/>
+        <v>799.19999999999993</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -1980,16 +1988,16 @@
         <v>35</v>
       </c>
       <c r="D17" s="20">
-        <f>$D$21*((100-C17)/100)</f>
-        <v>1154.4000000000001</v>
+        <f t="shared" si="1"/>
+        <v>1731.6000000000001</v>
       </c>
       <c r="E17" s="20">
         <f>D17/$D$20</f>
-        <v>1300</v>
+        <v>1950.0000000000002</v>
       </c>
       <c r="F17" s="20">
-        <f>$D$21*(C17/100)</f>
-        <v>621.59999999999991</v>
+        <f t="shared" si="2"/>
+        <v>932.4</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -2001,16 +2009,16 @@
         <v>40</v>
       </c>
       <c r="D18" s="20">
-        <f>$D$21*((100-C18)/100)</f>
-        <v>1065.5999999999999</v>
+        <f t="shared" si="1"/>
+        <v>1598.3999999999999</v>
       </c>
       <c r="E18" s="20">
         <f>D18/$D$20</f>
-        <v>1199.9999999999998</v>
+        <v>1799.9999999999998</v>
       </c>
       <c r="F18" s="20">
-        <f>$D$21*(C18/100)</f>
-        <v>710.40000000000009</v>
+        <f t="shared" si="2"/>
+        <v>1065.6000000000001</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -2050,8 +2058,15 @@
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="42"/>
+      <c r="A22" s="75"/>
+      <c r="B22" s="75"/>
+      <c r="D22" s="16">
+        <f>C2*D20</f>
+        <v>2664</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>76</v>
+      </c>
       <c r="J22" s="5" t="s">
         <v>99</v>
       </c>
@@ -2062,191 +2077,159 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="56">
+      <c r="B24" s="56">
         <v>0</v>
       </c>
-      <c r="C23" s="20">
-        <f>(F23/(D23+F23))*100</f>
-        <v>10.937761185713491</v>
-      </c>
-      <c r="D23" s="20">
-        <f>$D$20*E23</f>
-        <v>1598.4</v>
-      </c>
-      <c r="E23" s="20">
-        <v>1800</v>
-      </c>
-      <c r="F23" s="20">
-        <v>196.3</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="L23" s="58"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="60"/>
-      <c r="B24" s="56">
-        <v>1</v>
-      </c>
       <c r="C24" s="20">
-        <f t="shared" ref="C24:C27" si="1">(F24/(D24+F24))*100</f>
-        <v>14.075929193465766</v>
+        <f>(F24/(D24+F24))*100</f>
+        <v>0</v>
       </c>
       <c r="D24" s="20">
-        <f t="shared" ref="D24:D27" si="2">$D$20*E24</f>
-        <v>1509.6</v>
+        <f>$D$20*E24</f>
+        <v>2131.1999999999998</v>
       </c>
       <c r="E24" s="20">
-        <v>1700</v>
-      </c>
-      <c r="F24" s="20">
-        <v>247.3</v>
-      </c>
+        <v>2400</v>
+      </c>
+      <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
-      <c r="K24" s="67"/>
       <c r="L24" s="58"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="60"/>
       <c r="B25" s="56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="20">
-        <f t="shared" si="1"/>
-        <v>15.257662512630517</v>
+        <f t="shared" ref="C25:C28" si="3">(F25/(D25+F25))*100</f>
+        <v>0</v>
       </c>
       <c r="D25" s="20">
-        <f t="shared" si="2"/>
-        <v>1509.6</v>
+        <f t="shared" ref="D25:D28" si="4">$D$20*E25</f>
+        <v>1953.6000000000001</v>
       </c>
       <c r="E25" s="20">
-        <v>1700</v>
-      </c>
-      <c r="F25" s="20">
-        <v>271.8</v>
-      </c>
+        <v>2200</v>
+      </c>
+      <c r="F25" s="20"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
-      <c r="J25" s="67"/>
       <c r="K25" s="67"/>
       <c r="L25" s="58"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="60"/>
       <c r="B26" s="56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" s="20">
-        <f t="shared" si="1"/>
-        <v>17.295786993918806</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D26" s="20">
-        <f t="shared" si="2"/>
-        <v>1509.6</v>
+        <f t="shared" si="4"/>
+        <v>1864.8</v>
       </c>
       <c r="E26" s="20">
-        <v>1700</v>
-      </c>
-      <c r="F26" s="20">
-        <v>315.7</v>
-      </c>
+        <v>2100</v>
+      </c>
+      <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
       <c r="L26" s="58"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="60"/>
       <c r="B27" s="56">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D27" s="20">
-        <f t="shared" si="2"/>
-        <v>1420.8</v>
+        <f t="shared" si="4"/>
+        <v>1687.2</v>
       </c>
       <c r="E27" s="20">
-        <v>1600</v>
+        <v>1900</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-      <c r="K27" s="67"/>
       <c r="L27" s="58"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="42"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="60" t="s">
+      <c r="A28" s="60"/>
+      <c r="B28" s="56">
+        <v>4</v>
+      </c>
+      <c r="C28" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="20">
+        <f t="shared" si="4"/>
+        <v>1598.4</v>
+      </c>
+      <c r="E28" s="20">
+        <v>1800</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="58"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="42"/>
+      <c r="B29" s="42"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="56">
+      <c r="B30" s="56">
         <v>0</v>
       </c>
-      <c r="C29" s="20">
-        <f>(F29/(D29+F29))*100</f>
+      <c r="C30" s="20">
+        <f>(F30/(D30+F30))*100</f>
         <v>0.25833988543187686</v>
       </c>
-      <c r="D29" s="20">
-        <f>$D$20*E29</f>
+      <c r="D30" s="20">
+        <f>$D$20*E30</f>
         <v>1776</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E30" s="20">
         <v>2000</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F30" s="20">
         <v>4.5999999999999996</v>
-      </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="J29" s="4">
-        <v>2.6400000000000002E-4</v>
-      </c>
-      <c r="K29" s="4">
-        <v>1.7329999999999999E-3</v>
-      </c>
-      <c r="L29" s="58">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="60"/>
-      <c r="B30" s="56">
-        <v>1</v>
-      </c>
-      <c r="C30" s="20">
-        <f t="shared" ref="C30:C33" si="3">(F30/(D30+F30))*100</f>
-        <v>4.1635898892360119</v>
-      </c>
-      <c r="D30" s="20">
-        <f t="shared" ref="D30:D33" si="4">$D$20*E30</f>
-        <v>1687.2</v>
-      </c>
-      <c r="E30" s="20">
-        <v>1900</v>
-      </c>
-      <c r="F30" s="20">
-        <v>73.3</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="J30" s="4">
-        <v>2.9629999999999999E-3</v>
-      </c>
-      <c r="K30" s="67">
-        <v>0.95067100000000004</v>
+        <v>2.6400000000000002E-4</v>
+      </c>
+      <c r="K30" s="4">
+        <v>1.7329999999999999E-3</v>
       </c>
       <c r="L30" s="58">
         <v>20</v>
@@ -2255,29 +2238,29 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="60"/>
       <c r="B31" s="56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="20">
-        <f t="shared" si="3"/>
-        <v>8.3275980729525099</v>
+        <f t="shared" ref="C31:C34" si="5">(F31/(D31+F31))*100</f>
+        <v>4.1635898892360119</v>
       </c>
       <c r="D31" s="20">
-        <f t="shared" si="4"/>
-        <v>1598.4</v>
+        <f t="shared" ref="D31:D34" si="6">$D$20*E31</f>
+        <v>1687.2</v>
       </c>
       <c r="E31" s="20">
-        <v>1800</v>
+        <v>1900</v>
       </c>
       <c r="F31" s="20">
-        <v>145.19999999999999</v>
+        <v>73.3</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
-      <c r="J31" s="67">
-        <v>3.5182999999999999E-2</v>
+      <c r="J31" s="4">
+        <v>2.9629999999999999E-3</v>
       </c>
       <c r="K31" s="67">
-        <v>4.2918999999999999E-2</v>
+        <v>0.95067100000000004</v>
       </c>
       <c r="L31" s="58">
         <v>20</v>
@@ -2286,29 +2269,29 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="60"/>
       <c r="B32" s="56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="20">
-        <f t="shared" si="3"/>
-        <v>11.031949237448513</v>
+        <f t="shared" si="5"/>
+        <v>8.3275980729525099</v>
       </c>
       <c r="D32" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1598.4</v>
       </c>
       <c r="E32" s="20">
         <v>1800</v>
       </c>
       <c r="F32" s="20">
-        <v>198.2</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
-      <c r="J32" s="4">
-        <v>2.8964E-2</v>
-      </c>
-      <c r="K32" s="4">
-        <v>0.31996999999999998</v>
+      <c r="J32" s="67">
+        <v>3.5182999999999999E-2</v>
+      </c>
+      <c r="K32" s="67">
+        <v>4.2918999999999999E-2</v>
       </c>
       <c r="L32" s="58">
         <v>20</v>
@@ -2317,504 +2300,472 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="56">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" s="20">
-        <f t="shared" si="3"/>
-        <v>15.172902080219371</v>
+        <f t="shared" si="5"/>
+        <v>11.031949237448513</v>
       </c>
       <c r="D33" s="20">
-        <f t="shared" si="4"/>
-        <v>1509.6</v>
+        <f t="shared" si="6"/>
+        <v>1598.4</v>
       </c>
       <c r="E33" s="20">
-        <v>1700</v>
+        <v>1800</v>
       </c>
       <c r="F33" s="20">
-        <v>270.02</v>
+        <v>198.2</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="J33" s="4">
-        <v>0.198681</v>
-      </c>
-      <c r="K33" s="67">
-        <v>1.2781130000000001</v>
+        <v>2.8964E-2</v>
+      </c>
+      <c r="K33" s="4">
+        <v>0.31996999999999998</v>
       </c>
       <c r="L33" s="58">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="43"/>
-    </row>
-    <row r="35" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="59" t="s">
+      <c r="A34" s="60"/>
+      <c r="B34" s="56">
+        <v>4</v>
+      </c>
+      <c r="C34" s="20">
+        <f t="shared" si="5"/>
+        <v>15.172902080219371</v>
+      </c>
+      <c r="D34" s="20">
+        <f t="shared" si="6"/>
+        <v>1509.6</v>
+      </c>
+      <c r="E34" s="20">
+        <v>1700</v>
+      </c>
+      <c r="F34" s="20">
+        <v>270.02</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="J34" s="4">
+        <v>0.198681</v>
+      </c>
+      <c r="K34" s="67">
+        <v>1.2781130000000001</v>
+      </c>
+      <c r="L34" s="58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
+    </row>
+    <row r="36" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="31" t="s">
+      <c r="B36" s="53"/>
+      <c r="C36" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D36" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E36" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="H36" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="I35" s="36"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="15">
-        <v>9</v>
-      </c>
-      <c r="D36" s="20">
-        <f>$D$43*((100-C36)*0.75/100)</f>
-        <v>1233.2774999999999</v>
-      </c>
-      <c r="E36" s="20">
-        <f>D36/$D$42</f>
-        <v>1388.8260135135133</v>
-      </c>
-      <c r="F36" s="20">
-        <f>$D$43*((100-C36)*0.25/100)</f>
-        <v>411.09250000000003</v>
-      </c>
-      <c r="G36" s="20">
-        <f>F36/$F$42</f>
-        <v>432.72894736842113</v>
-      </c>
-      <c r="H36" s="20">
-        <f>$D$43*(C36/100)</f>
-        <v>162.63</v>
-      </c>
+      <c r="I36" s="36"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="59"/>
       <c r="B37" s="53"/>
       <c r="C37" s="15">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D37" s="20">
-        <f t="shared" ref="D37:D40" si="5">$D$43*((100-C37)*0.75/100)</f>
-        <v>1165.5150000000001</v>
+        <f>$D$45*((100-C37)*0.75/100)</f>
+        <v>1849.91625</v>
       </c>
       <c r="E37" s="20">
-        <f t="shared" ref="E37:E40" si="6">D37/$D$42</f>
-        <v>1312.5168918918921</v>
+        <f>D37/$D$43</f>
+        <v>2083.2390202702704</v>
       </c>
       <c r="F37" s="20">
-        <f t="shared" ref="F37:F40" si="7">$D$43*((100-C37)*0.25/100)</f>
-        <v>388.505</v>
+        <f>$D$45*((100-C37)*0.25/100)</f>
+        <v>616.63875000000007</v>
       </c>
       <c r="G37" s="20">
-        <f t="shared" ref="G37:G40" si="8">F37/$F$42</f>
-        <v>408.95263157894738</v>
+        <f>F37/$F$43</f>
+        <v>649.0934210526317</v>
       </c>
       <c r="H37" s="20">
-        <f t="shared" ref="H37:H40" si="9">$D$43*(C37/100)</f>
-        <v>252.98000000000002</v>
+        <f>$D$45*(C37/100)</f>
+        <v>243.94499999999999</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="59"/>
       <c r="B38" s="53"/>
       <c r="C38" s="15">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D38" s="20">
-        <f t="shared" si="5"/>
-        <v>1097.7525000000001</v>
+        <f t="shared" ref="D38:D41" si="7">$D$45*((100-C38)*0.75/100)</f>
+        <v>1748.2725</v>
       </c>
       <c r="E38" s="20">
-        <f t="shared" si="6"/>
-        <v>1236.2077702702702</v>
+        <f t="shared" ref="E38:E41" si="8">D38/$D$43</f>
+        <v>1968.7753378378379</v>
       </c>
       <c r="F38" s="20">
-        <f t="shared" si="7"/>
-        <v>365.91750000000002</v>
+        <f t="shared" ref="F38:F41" si="9">$D$45*((100-C38)*0.25/100)</f>
+        <v>582.75749999999994</v>
       </c>
       <c r="G38" s="20">
-        <f t="shared" si="8"/>
-        <v>385.17631578947373</v>
+        <f t="shared" ref="G38:G41" si="10">F38/$F$43</f>
+        <v>613.42894736842106</v>
       </c>
       <c r="H38" s="20">
-        <f t="shared" si="9"/>
-        <v>343.33</v>
+        <f t="shared" ref="H38:H41" si="11">$D$45*(C38/100)</f>
+        <v>379.47</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="59"/>
       <c r="B39" s="53"/>
       <c r="C39" s="15">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D39" s="20">
-        <f t="shared" si="5"/>
-        <v>1029.99</v>
+        <f t="shared" si="7"/>
+        <v>1646.6287500000001</v>
       </c>
       <c r="E39" s="20">
-        <f t="shared" si="6"/>
-        <v>1159.8986486486485</v>
+        <f t="shared" si="8"/>
+        <v>1854.3116554054054</v>
       </c>
       <c r="F39" s="20">
-        <f t="shared" si="7"/>
-        <v>343.33</v>
+        <f t="shared" si="9"/>
+        <v>548.87625000000003</v>
       </c>
       <c r="G39" s="20">
-        <f t="shared" si="8"/>
-        <v>361.4</v>
+        <f t="shared" si="10"/>
+        <v>577.76447368421054</v>
       </c>
       <c r="H39" s="20">
-        <f t="shared" si="9"/>
-        <v>433.68</v>
+        <f t="shared" si="11"/>
+        <v>514.995</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="59"/>
       <c r="B40" s="53"/>
       <c r="C40" s="15">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D40" s="20">
-        <f t="shared" si="5"/>
-        <v>962.22749999999996</v>
+        <f t="shared" si="7"/>
+        <v>1544.9849999999999</v>
       </c>
       <c r="E40" s="20">
-        <f t="shared" si="6"/>
-        <v>1083.5895270270269</v>
+        <f t="shared" si="8"/>
+        <v>1739.8479729729729</v>
       </c>
       <c r="F40" s="20">
-        <f t="shared" si="7"/>
-        <v>320.74250000000001</v>
+        <f t="shared" si="9"/>
+        <v>514.995</v>
       </c>
       <c r="G40" s="20">
-        <f t="shared" si="8"/>
-        <v>337.62368421052633</v>
+        <f t="shared" si="10"/>
+        <v>542.1</v>
       </c>
       <c r="H40" s="20">
-        <f t="shared" si="9"/>
-        <v>524.03</v>
+        <f t="shared" si="11"/>
+        <v>650.52</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
       <c r="B41" s="53"/>
+      <c r="C41" s="15">
+        <v>29</v>
+      </c>
+      <c r="D41" s="20">
+        <f t="shared" si="7"/>
+        <v>1443.3412499999999</v>
+      </c>
+      <c r="E41" s="20">
+        <f t="shared" si="8"/>
+        <v>1625.3842905405404</v>
+      </c>
+      <c r="F41" s="20">
+        <f t="shared" si="9"/>
+        <v>481.11374999999998</v>
+      </c>
+      <c r="G41" s="20">
+        <f t="shared" si="10"/>
+        <v>506.4355263157895</v>
+      </c>
+      <c r="H41" s="20">
+        <f t="shared" si="11"/>
+        <v>786.04499999999996</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="59"/>
       <c r="B42" s="53"/>
-      <c r="C42" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="45">
-        <v>0.88800000000000001</v>
-      </c>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45">
-        <v>0.95</v>
-      </c>
-      <c r="G42" s="20">
-        <v>1400</v>
-      </c>
-      <c r="H42" s="45">
-        <v>1.04</v>
-      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="59"/>
       <c r="B43" s="53"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16">
-        <f>C1*((D42*0.75)+(F42*0.25))</f>
+      <c r="C43" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="45">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45">
+        <v>0.95</v>
+      </c>
+      <c r="G43" s="20">
+        <v>1400</v>
+      </c>
+      <c r="H43" s="45">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="59"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16">
+        <f>C1*((D43*0.75)+(F43*0.25))</f>
         <v>1807</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E44" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J44" s="5" t="s">
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16">
+        <f>C2*((D43*0.75)+(F43*0.25))</f>
+        <v>2710.5</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J46" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="K44" s="5" t="s">
+      <c r="K46" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="L44" s="5" t="s">
+      <c r="L46" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="60" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="56">
+      <c r="B47" s="56">
         <v>5</v>
       </c>
-      <c r="C45" s="20">
-        <f>(H45/(D45+F45+H45))*100</f>
+      <c r="C47" s="20">
+        <f>(H47/(D47+F47+H47))*100</f>
         <v>0</v>
       </c>
-      <c r="D45" s="20">
-        <f>$D$42*E45</f>
-        <v>1243.2</v>
-      </c>
-      <c r="E45" s="20">
-        <v>1400</v>
-      </c>
-      <c r="F45" s="20">
-        <f>$F$42*G45</f>
-        <v>380</v>
-      </c>
-      <c r="G45" s="20">
-        <v>400</v>
-      </c>
-      <c r="H45" s="20"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="67"/>
-      <c r="L45" s="58"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="61"/>
-      <c r="B46" s="57">
-        <v>6</v>
-      </c>
-      <c r="C46" s="20">
-        <f t="shared" ref="C46:C48" si="10">(H46/(D46+F46+H46))*100</f>
-        <v>0</v>
-      </c>
-      <c r="D46" s="20">
-        <f t="shared" ref="D46" si="11">$D$42*E46</f>
-        <v>1154.4000000000001</v>
-      </c>
-      <c r="E46" s="20">
-        <v>1300</v>
-      </c>
-      <c r="F46" s="20">
-        <f t="shared" ref="F46:F48" si="12">$F$42*G46</f>
-        <v>380</v>
-      </c>
-      <c r="G46" s="20">
-        <v>400</v>
-      </c>
-      <c r="H46" s="20"/>
-      <c r="L46" s="58"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="61"/>
-      <c r="B47" s="57">
-        <v>7</v>
-      </c>
-      <c r="C47" s="20">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
       <c r="D47" s="20">
-        <v>1151</v>
+        <f>$D$43*E47</f>
+        <v>1864.8</v>
       </c>
       <c r="E47" s="20">
-        <v>1300</v>
+        <v>2100</v>
       </c>
       <c r="F47" s="20">
-        <v>383</v>
+        <f>$F$43*G47</f>
+        <v>570</v>
       </c>
       <c r="G47" s="20">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="H47" s="20"/>
-      <c r="J47" s="67"/>
+      <c r="J47" s="6"/>
       <c r="K47" s="67"/>
       <c r="L47" s="58"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="61"/>
       <c r="B48" s="57">
+        <v>6</v>
+      </c>
+      <c r="C48" s="20">
+        <f t="shared" ref="C48:C51" si="12">(H48/(D48+F48+H48))*100</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="20">
+        <f t="shared" ref="D48:D51" si="13">$D$43*E48</f>
+        <v>1776</v>
+      </c>
+      <c r="E48" s="20">
+        <v>2000</v>
+      </c>
+      <c r="F48" s="20">
+        <f t="shared" ref="F48:F51" si="14">$F$43*G48</f>
+        <v>570</v>
+      </c>
+      <c r="G48" s="20">
+        <v>600</v>
+      </c>
+      <c r="H48" s="20"/>
+      <c r="L48" s="58"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="61"/>
+      <c r="B49" s="57">
+        <v>7</v>
+      </c>
+      <c r="C49" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="D49" s="20">
+        <f t="shared" si="13"/>
+        <v>1598.4</v>
+      </c>
+      <c r="E49" s="20">
+        <v>1800</v>
+      </c>
+      <c r="F49" s="20">
+        <f t="shared" si="14"/>
+        <v>570</v>
+      </c>
+      <c r="G49" s="20">
+        <v>600</v>
+      </c>
+      <c r="H49" s="20"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="67"/>
+      <c r="L49" s="58"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="61"/>
+      <c r="B50" s="57">
         <v>8</v>
       </c>
-      <c r="C48" s="20">
-        <f t="shared" si="10"/>
+      <c r="C50" s="20">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D48" s="20">
-        <f t="shared" ref="D48" si="13">$D$42*E48</f>
-        <v>1154.4000000000001</v>
-      </c>
-      <c r="E48" s="20">
-        <v>1300</v>
-      </c>
-      <c r="F48" s="20">
-        <f t="shared" si="12"/>
-        <v>380</v>
-      </c>
-      <c r="G48" s="20">
-        <v>400</v>
-      </c>
-      <c r="H48" s="20"/>
-      <c r="J48" s="67"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="58"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="56">
-        <v>5</v>
-      </c>
-      <c r="C50" s="20">
-        <f>(H50/(D50+F50+H50))*100</f>
-        <v>1.4023026136301631</v>
-      </c>
       <c r="D50" s="20">
-        <f>$D$42*E50</f>
-        <v>1332</v>
+        <f t="shared" si="13"/>
+        <v>1509.6</v>
       </c>
       <c r="E50" s="20">
-        <v>1500</v>
+        <v>1700</v>
       </c>
       <c r="F50" s="20">
-        <f>$F$42*G50</f>
+        <f t="shared" si="14"/>
         <v>475</v>
       </c>
       <c r="G50" s="20">
         <v>500</v>
       </c>
-      <c r="H50" s="20">
-        <v>25.7</v>
-      </c>
-      <c r="J50" s="6">
-        <v>8.7530000000000004E-3</v>
-      </c>
-      <c r="K50" s="67">
-        <v>8.3807010000000002</v>
-      </c>
-      <c r="L50" s="58">
-        <v>20</v>
-      </c>
+      <c r="H50" s="20"/>
+      <c r="J50" s="67"/>
+      <c r="K50" s="67"/>
+      <c r="L50" s="58"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="61"/>
       <c r="B51" s="57">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C51" s="20">
-        <f t="shared" ref="C51:C54" si="14">(H51/(D51+F51+H51))*100</f>
-        <v>3.8727524204702628</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="D51" s="20">
-        <f t="shared" ref="D51:D54" si="15">$D$42*E51</f>
-        <v>1332</v>
+        <f t="shared" si="13"/>
+        <v>1420.8</v>
       </c>
       <c r="E51" s="20">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="F51" s="20">
-        <f t="shared" ref="F51:F54" si="16">$F$42*G51</f>
+        <f t="shared" si="14"/>
         <v>475</v>
       </c>
       <c r="G51" s="20">
         <v>500</v>
       </c>
-      <c r="H51" s="20">
-        <v>72.8</v>
-      </c>
-      <c r="J51" s="4">
-        <v>4.2900000000000004E-3</v>
-      </c>
-      <c r="K51" s="4">
-        <v>3.0336999999999999E-2</v>
-      </c>
-      <c r="L51" s="58">
-        <v>20</v>
-      </c>
+      <c r="H51" s="20"/>
+      <c r="J51" s="67"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="58"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="61"/>
-      <c r="B52" s="57">
-        <v>7</v>
-      </c>
-      <c r="C52" s="20">
-        <f t="shared" si="14"/>
-        <v>8.0392045776443251</v>
-      </c>
-      <c r="D52" s="20">
-        <f>$D$42*G42</f>
-        <v>1243.2</v>
-      </c>
-      <c r="E52" s="20">
-        <v>1400</v>
-      </c>
-      <c r="F52" s="20">
-        <f t="shared" si="16"/>
-        <v>380</v>
-      </c>
-      <c r="G52" s="20">
-        <v>400</v>
-      </c>
-      <c r="H52" s="20">
-        <v>141.9</v>
-      </c>
-      <c r="J52" s="67">
-        <v>1.9382E-2</v>
-      </c>
-      <c r="K52" s="67">
-        <v>0.236674</v>
-      </c>
-      <c r="L52" s="58">
-        <v>20</v>
-      </c>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="61"/>
-      <c r="B53" s="57">
-        <v>8</v>
+      <c r="A53" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="56">
+        <v>5</v>
       </c>
       <c r="C53" s="20">
-        <f t="shared" si="14"/>
-        <v>11.750158164145628</v>
+        <f>(H53/(D53+F53+H53))*100</f>
+        <v>1.4023026136301631</v>
       </c>
       <c r="D53" s="20">
-        <f t="shared" si="15"/>
-        <v>1154.4000000000001</v>
+        <f>$D$43*E53</f>
+        <v>1332</v>
       </c>
       <c r="E53" s="20">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="F53" s="20">
-        <f t="shared" si="16"/>
-        <v>380</v>
+        <f>$F$43*G53</f>
+        <v>475</v>
       </c>
       <c r="G53" s="20">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="H53" s="20">
-        <v>204.3</v>
-      </c>
-      <c r="J53" s="67">
-        <v>3.4037999999999999E-2</v>
-      </c>
-      <c r="K53" s="6">
-        <v>4.5269999999999998E-3</v>
+        <v>25.7</v>
+      </c>
+      <c r="J53" s="6">
+        <v>8.7530000000000004E-3</v>
+      </c>
+      <c r="K53" s="67">
+        <v>8.3807010000000002</v>
       </c>
       <c r="L53" s="58">
         <v>20</v>
@@ -2823,139 +2774,184 @@
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="61"/>
       <c r="B54" s="57">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C54" s="20">
-        <f t="shared" si="14"/>
-        <v>14.646492740724259</v>
+        <f t="shared" ref="C54:C57" si="15">(H54/(D54+F54+H54))*100</f>
+        <v>3.8727524204702628</v>
       </c>
       <c r="D54" s="20">
-        <f t="shared" si="15"/>
-        <v>1154.4000000000001</v>
+        <f t="shared" ref="D54:D57" si="16">$D$43*E54</f>
+        <v>1332</v>
       </c>
       <c r="E54" s="20">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="F54" s="20">
-        <f t="shared" si="16"/>
-        <v>380</v>
+        <f t="shared" ref="F54:F57" si="17">$F$43*G54</f>
+        <v>475</v>
       </c>
       <c r="G54" s="20">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="H54" s="20">
-        <v>263.3</v>
+        <v>72.8</v>
       </c>
       <c r="J54" s="4">
-        <v>6.9047999999999998E-2</v>
+        <v>4.2900000000000004E-3</v>
       </c>
       <c r="K54" s="4">
-        <v>9.5713000000000006E-2</v>
+        <v>3.0336999999999999E-2</v>
       </c>
       <c r="L54" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="59" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="61"/>
+      <c r="B55" s="57">
+        <v>7</v>
+      </c>
+      <c r="C55" s="20">
+        <f t="shared" si="15"/>
+        <v>8.0392045776443251</v>
+      </c>
+      <c r="D55" s="20">
+        <f>$D$43*G43</f>
+        <v>1243.2</v>
+      </c>
+      <c r="E55" s="20">
+        <v>1400</v>
+      </c>
+      <c r="F55" s="20">
+        <f t="shared" si="17"/>
+        <v>380</v>
+      </c>
+      <c r="G55" s="20">
+        <v>400</v>
+      </c>
+      <c r="H55" s="20">
+        <v>141.9</v>
+      </c>
+      <c r="J55" s="67">
+        <v>1.9382E-2</v>
+      </c>
+      <c r="K55" s="67">
+        <v>0.236674</v>
+      </c>
+      <c r="L55" s="58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="61"/>
+      <c r="B56" s="57">
+        <v>8</v>
+      </c>
+      <c r="C56" s="20">
+        <f t="shared" si="15"/>
+        <v>11.750158164145628</v>
+      </c>
+      <c r="D56" s="20">
+        <f t="shared" si="16"/>
+        <v>1154.4000000000001</v>
+      </c>
+      <c r="E56" s="20">
+        <v>1300</v>
+      </c>
+      <c r="F56" s="20">
+        <f t="shared" si="17"/>
+        <v>380</v>
+      </c>
+      <c r="G56" s="20">
+        <v>400</v>
+      </c>
+      <c r="H56" s="20">
+        <v>204.3</v>
+      </c>
+      <c r="J56" s="67">
+        <v>3.4037999999999999E-2</v>
+      </c>
+      <c r="K56" s="6">
+        <v>4.5269999999999998E-3</v>
+      </c>
+      <c r="L56" s="58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="61"/>
+      <c r="B57" s="57">
+        <v>9</v>
+      </c>
+      <c r="C57" s="20">
+        <f t="shared" si="15"/>
+        <v>14.646492740724259</v>
+      </c>
+      <c r="D57" s="20">
+        <f t="shared" si="16"/>
+        <v>1154.4000000000001</v>
+      </c>
+      <c r="E57" s="20">
+        <v>1300</v>
+      </c>
+      <c r="F57" s="20">
+        <f t="shared" si="17"/>
+        <v>380</v>
+      </c>
+      <c r="G57" s="20">
+        <v>400</v>
+      </c>
+      <c r="H57" s="20">
+        <v>263.3</v>
+      </c>
+      <c r="J57" s="4">
+        <v>6.9047999999999998E-2</v>
+      </c>
+      <c r="K57" s="4">
+        <v>9.5713000000000006E-2</v>
+      </c>
+      <c r="L57" s="58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="B56" s="53"/>
-      <c r="C56" s="31" t="s">
+      <c r="B59" s="53"/>
+      <c r="C59" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D59" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F59" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G56" s="17"/>
-      <c r="I56" s="36"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="59"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="15">
-        <v>9</v>
-      </c>
-      <c r="D57" s="20">
-        <f>$D$64*((100-C57)/100)</f>
-        <v>1869.14</v>
-      </c>
-      <c r="E57" s="20">
-        <f>D57/$D$63</f>
-        <v>1820.0000000000002</v>
-      </c>
-      <c r="F57" s="20">
-        <f>$D$64*(C57/100)</f>
-        <v>184.85999999999999</v>
-      </c>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="59"/>
-      <c r="B58" s="53"/>
-      <c r="C58" s="15">
-        <v>14</v>
-      </c>
-      <c r="D58" s="20">
-        <f t="shared" ref="D58:D61" si="17">$D$64*((100-C58)/100)</f>
-        <v>1766.44</v>
-      </c>
-      <c r="E58" s="20">
-        <f t="shared" ref="E58:E61" si="18">D58/$D$63</f>
-        <v>1720.0000000000002</v>
-      </c>
-      <c r="F58" s="20">
-        <f t="shared" ref="F58:F61" si="19">$D$64*(C58/100)</f>
-        <v>287.56</v>
-      </c>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="59"/>
-      <c r="B59" s="53"/>
-      <c r="C59" s="15">
-        <v>19</v>
-      </c>
-      <c r="D59" s="20">
-        <f t="shared" si="17"/>
-        <v>1663.74</v>
-      </c>
-      <c r="E59" s="20">
-        <f t="shared" si="18"/>
-        <v>1620.0000000000002</v>
-      </c>
-      <c r="F59" s="20">
-        <f t="shared" si="19"/>
-        <v>390.26</v>
-      </c>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
+      <c r="G59" s="17"/>
+      <c r="I59" s="36"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="59"/>
       <c r="B60" s="53"/>
       <c r="C60" s="15">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D60" s="20">
-        <f t="shared" si="17"/>
-        <v>1561.04</v>
+        <f>$D$68*((100-C60)/100)</f>
+        <v>2803.7099999999996</v>
       </c>
       <c r="E60" s="20">
-        <f t="shared" si="18"/>
-        <v>1520</v>
+        <f>D60/$D$66</f>
+        <v>2730</v>
       </c>
       <c r="F60" s="20">
-        <f t="shared" si="19"/>
-        <v>492.96</v>
+        <f>$D$68*(C60/100)</f>
+        <v>277.28999999999996</v>
       </c>
       <c r="G60" s="20"/>
       <c r="H60" s="20"/>
@@ -2964,19 +2960,19 @@
       <c r="A61" s="59"/>
       <c r="B61" s="53"/>
       <c r="C61" s="15">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="D61" s="20">
-        <f t="shared" si="17"/>
-        <v>1458.34</v>
+        <f t="shared" ref="D61:D64" si="18">$D$68*((100-C61)/100)</f>
+        <v>2649.6599999999994</v>
       </c>
       <c r="E61" s="20">
-        <f t="shared" si="18"/>
-        <v>1420</v>
+        <f t="shared" ref="E61:E64" si="19">D61/$D$66</f>
+        <v>2579.9999999999995</v>
       </c>
       <c r="F61" s="20">
-        <f t="shared" si="19"/>
-        <v>595.66</v>
+        <f t="shared" ref="F61:F64" si="20">$D$68*(C61/100)</f>
+        <v>431.34</v>
       </c>
       <c r="G61" s="20"/>
       <c r="H61" s="20"/>
@@ -2984,1301 +2980,1401 @@
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="59"/>
       <c r="B62" s="53"/>
+      <c r="C62" s="15">
+        <v>19</v>
+      </c>
+      <c r="D62" s="20">
+        <f t="shared" si="18"/>
+        <v>2495.6099999999997</v>
+      </c>
+      <c r="E62" s="20">
+        <f t="shared" si="19"/>
+        <v>2430</v>
+      </c>
+      <c r="F62" s="20">
+        <f t="shared" si="20"/>
+        <v>585.38999999999987</v>
+      </c>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="59"/>
       <c r="B63" s="53"/>
-      <c r="C63" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D63" s="16">
-        <v>1.0269999999999999</v>
-      </c>
-      <c r="E63" s="16"/>
-      <c r="F63" s="45">
-        <v>1.04</v>
-      </c>
-      <c r="G63" s="45"/>
-      <c r="H63" s="16"/>
+      <c r="C63" s="15">
+        <v>24</v>
+      </c>
+      <c r="D63" s="20">
+        <f t="shared" si="18"/>
+        <v>2341.5599999999995</v>
+      </c>
+      <c r="E63" s="20">
+        <f t="shared" si="19"/>
+        <v>2279.9999999999995</v>
+      </c>
+      <c r="F63" s="20">
+        <f t="shared" si="20"/>
+        <v>739.43999999999983</v>
+      </c>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="59"/>
       <c r="B64" s="53"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16">
-        <f>C1*D63</f>
+      <c r="C64" s="15">
+        <v>29</v>
+      </c>
+      <c r="D64" s="20">
+        <f t="shared" si="18"/>
+        <v>2187.5099999999998</v>
+      </c>
+      <c r="E64" s="20">
+        <f t="shared" si="19"/>
+        <v>2130</v>
+      </c>
+      <c r="F64" s="20">
+        <f t="shared" si="20"/>
+        <v>893.48999999999978</v>
+      </c>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="59"/>
+      <c r="B65" s="53"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="59"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D66" s="16">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="E66" s="16"/>
+      <c r="F66" s="45">
+        <v>1.04</v>
+      </c>
+      <c r="G66" s="45"/>
+      <c r="H66" s="16"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="59"/>
+      <c r="B67" s="53"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16">
+        <f>C1*D66</f>
         <v>2054</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="E67" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="50"/>
-      <c r="B65" s="50"/>
-      <c r="C65" s="41"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6"/>
-      <c r="J65" s="5" t="s">
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="53"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16">
+        <f>C2*D66</f>
+        <v>3080.9999999999995</v>
+      </c>
+      <c r="E68" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="50"/>
+      <c r="B69" s="50"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="J69" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="K65" s="5" t="s">
+      <c r="K69" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="L65" s="5" t="s">
+      <c r="L69" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="62" t="s">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="B66" s="54">
-        <v>9</v>
-      </c>
-      <c r="C66" s="51">
-        <f>(F66/(D66+F66))*100</f>
+      <c r="B70" s="54">
+        <v>10</v>
+      </c>
+      <c r="C70" s="51">
+        <f>(F70/(D70+F70))*100</f>
         <v>0</v>
       </c>
-      <c r="D66" s="52">
-        <f>$D$63*E66</f>
-        <v>1848.6</v>
-      </c>
-      <c r="E66" s="52">
-        <v>1800</v>
-      </c>
-      <c r="F66" s="52"/>
-      <c r="G66" s="52"/>
-      <c r="H66" s="52"/>
-      <c r="K66" s="67"/>
-      <c r="L66" s="58"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="63"/>
-      <c r="B67" s="55">
-        <v>10</v>
-      </c>
-      <c r="C67" s="51">
-        <f t="shared" ref="C67:C69" si="20">(F67/(D67+F67))*100</f>
+      <c r="D70" s="52">
+        <f>$D$66*E70</f>
+        <v>2772.8999999999996</v>
+      </c>
+      <c r="E70" s="52">
+        <v>2700</v>
+      </c>
+      <c r="F70" s="52"/>
+      <c r="G70" s="52"/>
+      <c r="H70" s="52"/>
+      <c r="K70" s="67"/>
+      <c r="L70" s="58"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="63"/>
+      <c r="B71" s="55">
+        <v>11</v>
+      </c>
+      <c r="C71" s="51">
+        <f t="shared" ref="C71:C74" si="21">(F71/(D71+F71))*100</f>
         <v>0</v>
       </c>
-      <c r="D67" s="52">
-        <f t="shared" ref="D67:D69" si="21">$D$63*E67</f>
-        <v>1745.8999999999999</v>
-      </c>
-      <c r="E67" s="52">
-        <v>1700</v>
-      </c>
-      <c r="F67" s="52"/>
-      <c r="G67" s="52"/>
-      <c r="H67" s="52"/>
-      <c r="L67" s="58"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="63"/>
-      <c r="B68" s="55">
-        <v>11</v>
-      </c>
-      <c r="C68" s="51">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="D68" s="52">
-        <f t="shared" si="21"/>
-        <v>1745.8999999999999</v>
-      </c>
-      <c r="E68" s="52">
-        <v>1700</v>
-      </c>
-      <c r="F68" s="52"/>
-      <c r="G68" s="52"/>
-      <c r="H68" s="52"/>
-      <c r="K68" s="67"/>
-      <c r="L68" s="58"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="63"/>
-      <c r="B69" s="55">
-        <v>12</v>
-      </c>
-      <c r="C69" s="51">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="D69" s="52">
-        <f t="shared" si="21"/>
-        <v>1745.8999999999999</v>
-      </c>
-      <c r="E69" s="52">
-        <v>1700</v>
-      </c>
-      <c r="F69" s="52"/>
-      <c r="G69" s="52"/>
-      <c r="H69" s="52"/>
-      <c r="L69" s="58"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="50"/>
-      <c r="B70" s="50"/>
-      <c r="C70" s="41"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="B71" s="54">
-        <v>10</v>
-      </c>
-      <c r="C71" s="51">
-        <f>(F71/(D71+F71))*100</f>
-        <v>1.0263576350407171</v>
-      </c>
       <c r="D71" s="52">
-        <f>$D$63*E71</f>
-        <v>2054</v>
+        <f>$D$66*E71</f>
+        <v>2670.2</v>
       </c>
       <c r="E71" s="52">
-        <v>2000</v>
-      </c>
-      <c r="F71" s="52">
-        <v>21.3</v>
-      </c>
+        <v>2600</v>
+      </c>
+      <c r="F71" s="52"/>
       <c r="G71" s="52"/>
       <c r="H71" s="52"/>
-      <c r="J71" s="4">
-        <v>2.0917000000000002E-2</v>
-      </c>
-      <c r="K71" s="67">
-        <v>53.570850999999998</v>
-      </c>
-      <c r="L71" s="58">
-        <v>20</v>
-      </c>
+      <c r="L71" s="58"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="63"/>
       <c r="B72" s="55">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C72" s="51">
-        <f t="shared" ref="C72:C75" si="22">(F72/(D72+F72))*100</f>
-        <v>3.5633092814075318</v>
+        <f t="shared" si="21"/>
+        <v>0</v>
       </c>
       <c r="D72" s="52">
-        <f t="shared" ref="D72:D75" si="23">$D$63*E72</f>
-        <v>1951.2999999999997</v>
+        <f>$D$66*E72</f>
+        <v>2464.7999999999997</v>
       </c>
       <c r="E72" s="52">
-        <v>1900</v>
-      </c>
-      <c r="F72" s="52">
-        <v>72.099999999999994</v>
-      </c>
+        <v>2400</v>
+      </c>
+      <c r="F72" s="52"/>
       <c r="G72" s="52"/>
       <c r="H72" s="52"/>
-      <c r="J72" s="4">
-        <v>9.1500000000000001E-3</v>
-      </c>
-      <c r="K72" s="4">
-        <v>2.2258E-2</v>
-      </c>
-      <c r="L72" s="58">
-        <v>20</v>
-      </c>
+      <c r="K72" s="67"/>
+      <c r="L72" s="58"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="63"/>
       <c r="B73" s="55">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C73" s="51">
-        <f t="shared" si="22"/>
-        <v>7.74067974247642</v>
+        <f t="shared" si="21"/>
+        <v>0</v>
       </c>
       <c r="D73" s="52">
-        <f t="shared" si="23"/>
-        <v>1848.6</v>
+        <f>$D$66*E73</f>
+        <v>2362.1</v>
       </c>
       <c r="E73" s="52">
-        <v>1800</v>
-      </c>
-      <c r="F73" s="52">
-        <v>155.1</v>
-      </c>
+        <v>2300</v>
+      </c>
+      <c r="F73" s="52"/>
       <c r="G73" s="52"/>
       <c r="H73" s="52"/>
-      <c r="J73" s="4">
-        <v>3.1720999999999999E-2</v>
-      </c>
-      <c r="K73" s="67">
-        <v>2.6790000000000001E-2</v>
-      </c>
-      <c r="L73" s="58">
-        <v>20</v>
-      </c>
+      <c r="K73" s="67"/>
+      <c r="L73" s="58"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="63"/>
       <c r="B74" s="55">
+        <v>14</v>
+      </c>
+      <c r="C74" s="51">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="D74" s="52">
+        <f>$D$66*E74</f>
+        <v>2156.6999999999998</v>
+      </c>
+      <c r="E74" s="52">
+        <v>2100</v>
+      </c>
+      <c r="F74" s="52"/>
+      <c r="G74" s="52"/>
+      <c r="H74" s="52"/>
+      <c r="L74" s="58"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="50"/>
+      <c r="B75" s="50"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="B76" s="54">
+        <v>10</v>
+      </c>
+      <c r="C76" s="51">
+        <f>(F76/(D76+F76))*100</f>
+        <v>1.0263576350407171</v>
+      </c>
+      <c r="D76" s="52">
+        <f>$D$66*E76</f>
+        <v>2054</v>
+      </c>
+      <c r="E76" s="52">
+        <v>2000</v>
+      </c>
+      <c r="F76" s="52">
+        <v>21.3</v>
+      </c>
+      <c r="G76" s="52"/>
+      <c r="H76" s="52"/>
+      <c r="J76" s="4">
+        <v>2.0917000000000002E-2</v>
+      </c>
+      <c r="K76" s="67">
+        <v>53.570850999999998</v>
+      </c>
+      <c r="L76" s="58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="63"/>
+      <c r="B77" s="55">
+        <v>11</v>
+      </c>
+      <c r="C77" s="51">
+        <f t="shared" ref="C77:C80" si="22">(F77/(D77+F77))*100</f>
+        <v>3.5633092814075318</v>
+      </c>
+      <c r="D77" s="52">
+        <f t="shared" ref="D77:D80" si="23">$D$66*E77</f>
+        <v>1951.2999999999997</v>
+      </c>
+      <c r="E77" s="52">
+        <v>1900</v>
+      </c>
+      <c r="F77" s="52">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="G77" s="52"/>
+      <c r="H77" s="52"/>
+      <c r="J77" s="4">
+        <v>9.1500000000000001E-3</v>
+      </c>
+      <c r="K77" s="4">
+        <v>2.2258E-2</v>
+      </c>
+      <c r="L77" s="58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="63"/>
+      <c r="B78" s="55">
+        <v>12</v>
+      </c>
+      <c r="C78" s="51">
+        <f t="shared" si="22"/>
+        <v>7.74067974247642</v>
+      </c>
+      <c r="D78" s="52">
+        <f t="shared" si="23"/>
+        <v>1848.6</v>
+      </c>
+      <c r="E78" s="52">
+        <v>1800</v>
+      </c>
+      <c r="F78" s="52">
+        <v>155.1</v>
+      </c>
+      <c r="G78" s="52"/>
+      <c r="H78" s="52"/>
+      <c r="J78" s="4">
+        <v>3.1720999999999999E-2</v>
+      </c>
+      <c r="K78" s="67">
+        <v>2.6790000000000001E-2</v>
+      </c>
+      <c r="L78" s="58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="63"/>
+      <c r="B79" s="55">
         <v>13</v>
       </c>
-      <c r="C74" s="51">
+      <c r="C79" s="51">
         <f t="shared" si="22"/>
         <v>11.512134411947729</v>
       </c>
-      <c r="D74" s="52">
+      <c r="D79" s="52">
         <f t="shared" si="23"/>
         <v>1848.6</v>
       </c>
-      <c r="E74" s="52">
+      <c r="E79" s="52">
         <v>1800</v>
       </c>
-      <c r="F74" s="52">
+      <c r="F79" s="52">
         <v>240.5</v>
       </c>
-      <c r="G74" s="52"/>
-      <c r="H74" s="52"/>
-      <c r="J74" s="4">
+      <c r="G79" s="52"/>
+      <c r="H79" s="52"/>
+      <c r="J79" s="4">
         <v>8.6243E-2</v>
       </c>
-      <c r="K74" s="4">
+      <c r="K79" s="4">
         <v>1.5518959999999999</v>
       </c>
-      <c r="L74" s="58">
+      <c r="L79" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="63"/>
-      <c r="B75" s="55">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="63"/>
+      <c r="B80" s="55">
         <v>14</v>
       </c>
-      <c r="C75" s="51">
+      <c r="C80" s="51">
         <f t="shared" si="22"/>
         <v>14.950311769290725</v>
       </c>
-      <c r="D75" s="52">
+      <c r="D80" s="52">
         <f t="shared" si="23"/>
         <v>1745.8999999999999</v>
       </c>
-      <c r="E75" s="52">
+      <c r="E80" s="52">
         <v>1700</v>
       </c>
-      <c r="F75" s="52">
+      <c r="F80" s="52">
         <v>306.89999999999998</v>
       </c>
-      <c r="G75" s="52"/>
-      <c r="H75" s="52"/>
-      <c r="J75" s="4">
+      <c r="G80" s="52"/>
+      <c r="H80" s="52"/>
+      <c r="J80" s="4">
         <v>0.15590399999999999</v>
       </c>
-      <c r="K75" s="67">
+      <c r="K80" s="67">
         <v>0.16277</v>
       </c>
-      <c r="L75" s="58">
+      <c r="L80" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="59" t="s">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="B77" s="53"/>
-      <c r="C77" s="31" t="s">
+      <c r="B82" s="53"/>
+      <c r="C82" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="D77" s="26" t="s">
+      <c r="D82" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="E77" s="26" t="s">
+      <c r="E82" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F77" s="26" t="s">
+      <c r="F82" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="G77" s="26" t="s">
+      <c r="G82" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="H77" s="39"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="59"/>
-      <c r="B78" s="53"/>
-      <c r="C78" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="D78" s="28">
-        <f t="shared" ref="D78:D79" si="24">$D$85*((100-C78)/100)</f>
-        <v>2048.8650000000002</v>
-      </c>
-      <c r="E78" s="28">
-        <f>D78/$D$84</f>
-        <v>1995.0000000000005</v>
-      </c>
-      <c r="F78" s="28">
-        <f>$D$85*((C78*0.3)/100)</f>
-        <v>1.5405</v>
-      </c>
-      <c r="G78" s="28">
-        <f>$D$85*((C78*0.7)/100)</f>
-        <v>3.5944999999999996</v>
-      </c>
-      <c r="H78" s="39"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="59"/>
-      <c r="B79" s="53"/>
-      <c r="C79" s="30">
-        <v>3.75</v>
-      </c>
-      <c r="D79" s="28">
-        <f t="shared" si="24"/>
-        <v>1976.9750000000001</v>
-      </c>
-      <c r="E79" s="28">
-        <f t="shared" ref="E79:E82" si="25">D79/$D$84</f>
-        <v>1925.0000000000002</v>
-      </c>
-      <c r="F79" s="28">
-        <f t="shared" ref="F79:F82" si="26">$D$85*((C79*0.3)/100)</f>
-        <v>23.107499999999998</v>
-      </c>
-      <c r="G79" s="28">
-        <f>$D$85*((C79*0.7)/100)</f>
-        <v>53.917499999999997</v>
-      </c>
-      <c r="H79" s="39"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="59"/>
-      <c r="B80" s="53"/>
-      <c r="C80" s="30">
-        <v>7.5</v>
-      </c>
-      <c r="D80" s="28">
-        <f>$D$85*((100-C80)/100)</f>
-        <v>1899.95</v>
-      </c>
-      <c r="E80" s="28">
-        <f t="shared" si="25"/>
-        <v>1850.0000000000002</v>
-      </c>
-      <c r="F80" s="28">
-        <f t="shared" si="26"/>
-        <v>46.214999999999996</v>
-      </c>
-      <c r="G80" s="28">
-        <f>$D$85*((C80*0.7)/100)</f>
-        <v>107.83499999999999</v>
-      </c>
-      <c r="H80" s="39"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="59"/>
-      <c r="B81" s="53"/>
-      <c r="C81" s="30">
-        <v>11.25</v>
-      </c>
-      <c r="D81" s="28">
-        <f t="shared" ref="D81:D82" si="27">$D$85*((100-C81)/100)</f>
-        <v>1822.925</v>
-      </c>
-      <c r="E81" s="28">
-        <f t="shared" si="25"/>
-        <v>1775</v>
-      </c>
-      <c r="F81" s="28">
-        <f t="shared" si="26"/>
-        <v>69.322500000000005</v>
-      </c>
-      <c r="G81" s="28">
-        <f>$D$85*((C81*0.7)/100)</f>
-        <v>161.75249999999997</v>
-      </c>
-      <c r="H81" s="39"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" s="59"/>
-      <c r="B82" s="53"/>
-      <c r="C82" s="30">
-        <v>15</v>
-      </c>
-      <c r="D82" s="28">
-        <f t="shared" si="27"/>
-        <v>1745.8999999999999</v>
-      </c>
-      <c r="E82" s="28">
-        <f t="shared" si="25"/>
-        <v>1700</v>
-      </c>
-      <c r="F82" s="28">
-        <f t="shared" si="26"/>
-        <v>92.429999999999993</v>
-      </c>
-      <c r="G82" s="28">
-        <f>$D$85*((C82*0.7)/100)</f>
-        <v>215.67</v>
-      </c>
       <c r="H82" s="39"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="59"/>
       <c r="B83" s="53"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
+      <c r="C83" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="D83" s="28">
+        <f t="shared" ref="D83:D84" si="24">$D$90*((100-C83)/100)</f>
+        <v>2048.8650000000002</v>
+      </c>
+      <c r="E83" s="28">
+        <f>D83/$D$89</f>
+        <v>1995.0000000000005</v>
+      </c>
+      <c r="F83" s="28">
+        <f>$D$90*((C83*0.3)/100)</f>
+        <v>1.5405</v>
+      </c>
+      <c r="G83" s="28">
+        <f>$D$90*((C83*0.7)/100)</f>
+        <v>3.5944999999999996</v>
+      </c>
       <c r="H83" s="39"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="59"/>
       <c r="B84" s="53"/>
-      <c r="C84" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="D84" s="48">
-        <v>1.0269999999999999</v>
-      </c>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48">
-        <v>1.2450000000000001</v>
-      </c>
-      <c r="G84" s="25">
-        <v>1.1839999999999999</v>
-      </c>
-      <c r="H84" s="49"/>
+      <c r="C84" s="30">
+        <v>3.75</v>
+      </c>
+      <c r="D84" s="28">
+        <f t="shared" si="24"/>
+        <v>1976.9750000000001</v>
+      </c>
+      <c r="E84" s="28">
+        <f t="shared" ref="E84:E87" si="25">D84/$D$89</f>
+        <v>1925.0000000000002</v>
+      </c>
+      <c r="F84" s="28">
+        <f t="shared" ref="F84:F87" si="26">$D$90*((C84*0.3)/100)</f>
+        <v>23.107499999999998</v>
+      </c>
+      <c r="G84" s="28">
+        <f>$D$90*((C84*0.7)/100)</f>
+        <v>53.917499999999997</v>
+      </c>
+      <c r="H84" s="39"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="59"/>
       <c r="B85" s="53"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25">
-        <f>C1*D84</f>
-        <v>2054</v>
-      </c>
-      <c r="E85" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="F85" s="25"/>
-      <c r="G85" s="25"/>
-      <c r="H85" s="25"/>
-    </row>
-    <row r="87" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="59" t="s">
-        <v>97</v>
-      </c>
+      <c r="C85" s="30">
+        <v>7.5</v>
+      </c>
+      <c r="D85" s="28">
+        <f>$D$90*((100-C85)/100)</f>
+        <v>1899.95</v>
+      </c>
+      <c r="E85" s="28">
+        <f t="shared" si="25"/>
+        <v>1850.0000000000002</v>
+      </c>
+      <c r="F85" s="28">
+        <f t="shared" si="26"/>
+        <v>46.214999999999996</v>
+      </c>
+      <c r="G85" s="28">
+        <f>$D$90*((C85*0.7)/100)</f>
+        <v>107.83499999999999</v>
+      </c>
+      <c r="H85" s="39"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="59"/>
+      <c r="B86" s="53"/>
+      <c r="C86" s="30">
+        <v>11.25</v>
+      </c>
+      <c r="D86" s="28">
+        <f t="shared" ref="D86:D87" si="27">$D$90*((100-C86)/100)</f>
+        <v>1822.925</v>
+      </c>
+      <c r="E86" s="28">
+        <f t="shared" si="25"/>
+        <v>1775</v>
+      </c>
+      <c r="F86" s="28">
+        <f t="shared" si="26"/>
+        <v>69.322500000000005</v>
+      </c>
+      <c r="G86" s="28">
+        <f>$D$90*((C86*0.7)/100)</f>
+        <v>161.75249999999997</v>
+      </c>
+      <c r="H86" s="39"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="59"/>
       <c r="B87" s="53"/>
-      <c r="C87" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G87" s="70"/>
-      <c r="H87" s="70"/>
-      <c r="I87" s="36"/>
+      <c r="C87" s="30">
+        <v>15</v>
+      </c>
+      <c r="D87" s="28">
+        <f t="shared" si="27"/>
+        <v>1745.8999999999999</v>
+      </c>
+      <c r="E87" s="28">
+        <f t="shared" si="25"/>
+        <v>1700</v>
+      </c>
+      <c r="F87" s="28">
+        <f t="shared" si="26"/>
+        <v>92.429999999999993</v>
+      </c>
+      <c r="G87" s="28">
+        <f>$D$90*((C87*0.7)/100)</f>
+        <v>215.67</v>
+      </c>
+      <c r="H87" s="39"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="59"/>
       <c r="B88" s="53"/>
-      <c r="C88" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D88" s="20">
-        <f>$D$95*((100-C88)/100)</f>
-        <v>2958.9840000000004</v>
-      </c>
-      <c r="E88" s="20">
-        <f>D88/$D$94</f>
-        <v>1995.0000000000002</v>
-      </c>
-      <c r="F88" s="20">
-        <f>$D$95*(C88/100)</f>
-        <v>7.4160000000000004</v>
-      </c>
-      <c r="G88" s="74"/>
-      <c r="H88" s="68"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="27"/>
+      <c r="H88" s="39"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="59"/>
       <c r="B89" s="53"/>
-      <c r="C89" s="30">
-        <v>3.75</v>
-      </c>
-      <c r="D89" s="38">
-        <f>$D$95*((100-C89)/100)</f>
-        <v>2855.1600000000003</v>
-      </c>
-      <c r="E89" s="20">
-        <f>D89/$D$94</f>
-        <v>1925</v>
-      </c>
-      <c r="F89" s="38">
-        <f>$D$95*(C89/100)</f>
-        <v>111.24</v>
-      </c>
-      <c r="G89" s="68"/>
-      <c r="H89" s="68"/>
+      <c r="C89" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="D89" s="48">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="E89" s="48"/>
+      <c r="F89" s="48">
+        <v>1.2450000000000001</v>
+      </c>
+      <c r="G89" s="25">
+        <v>1.1839999999999999</v>
+      </c>
+      <c r="H89" s="49"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="59"/>
       <c r="B90" s="53"/>
-      <c r="C90" s="15">
-        <v>7.5</v>
-      </c>
-      <c r="D90" s="20">
-        <f>$D$95*((100-C90)/100)</f>
-        <v>2743.92</v>
-      </c>
-      <c r="E90" s="20">
-        <f>D90/$D$94</f>
-        <v>1850</v>
-      </c>
-      <c r="F90" s="20">
-        <f>$D$95*(C90/100)</f>
-        <v>222.48</v>
-      </c>
-      <c r="G90" s="68"/>
-      <c r="H90" s="68"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" s="59"/>
-      <c r="B91" s="53"/>
-      <c r="C91" s="30">
-        <v>11.25</v>
-      </c>
-      <c r="D91" s="38">
-        <f>$D$95*((100-C91)/100)</f>
-        <v>2632.68</v>
-      </c>
-      <c r="E91" s="20">
-        <f>D91/$D$94</f>
-        <v>1774.9999999999998</v>
-      </c>
-      <c r="F91" s="38">
-        <f>$D$95*(C91/100)</f>
-        <v>333.72</v>
-      </c>
-      <c r="G91" s="71"/>
-      <c r="H91" s="68"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" s="59"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="25">
+        <f>C1*D89</f>
+        <v>2054</v>
+      </c>
+      <c r="E90" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F90" s="25"/>
+      <c r="G90" s="25"/>
+      <c r="H90" s="25"/>
+    </row>
+    <row r="92" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="59" t="s">
+        <v>97</v>
+      </c>
       <c r="B92" s="53"/>
-      <c r="C92" s="15">
-        <v>15</v>
-      </c>
-      <c r="D92" s="20">
-        <f>$D$95*((100-C92)/100)</f>
-        <v>2521.44</v>
-      </c>
-      <c r="E92" s="20">
-        <f>D92/$D$94</f>
-        <v>1700</v>
-      </c>
-      <c r="F92" s="20">
-        <f>$D$95*(C92/100)</f>
-        <v>444.96</v>
-      </c>
-      <c r="G92" s="71"/>
-      <c r="H92" s="68"/>
+      <c r="C92" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G92" s="70"/>
+      <c r="H92" s="70"/>
+      <c r="I92" s="36"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="59"/>
       <c r="B93" s="53"/>
-      <c r="G93" s="69"/>
-      <c r="H93" s="69"/>
+      <c r="C93" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="D93" s="20">
+        <f>$D$100*((100-C93)/100)</f>
+        <v>2958.9840000000004</v>
+      </c>
+      <c r="E93" s="20">
+        <f>D93/$D$99</f>
+        <v>1995.0000000000002</v>
+      </c>
+      <c r="F93" s="20">
+        <f>$D$100*(C93/100)</f>
+        <v>7.4160000000000004</v>
+      </c>
+      <c r="G93" s="74"/>
+      <c r="H93" s="68"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="59"/>
       <c r="B94" s="53"/>
-      <c r="C94" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D94" s="45">
-        <v>1.4832000000000001</v>
-      </c>
-      <c r="E94" s="45"/>
-      <c r="F94" s="45">
-        <v>1.2</v>
-      </c>
-      <c r="G94" s="72"/>
-      <c r="H94" s="73"/>
+      <c r="C94" s="30">
+        <v>3.75</v>
+      </c>
+      <c r="D94" s="38">
+        <f>$D$100*((100-C94)/100)</f>
+        <v>2855.1600000000003</v>
+      </c>
+      <c r="E94" s="20">
+        <f>D94/$D$99</f>
+        <v>1925</v>
+      </c>
+      <c r="F94" s="38">
+        <f>$D$100*(C94/100)</f>
+        <v>111.24</v>
+      </c>
+      <c r="G94" s="68"/>
+      <c r="H94" s="68"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="59"/>
       <c r="B95" s="53"/>
-      <c r="C95" s="16"/>
-      <c r="D95" s="16">
-        <f>C1*D94</f>
+      <c r="C95" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="D95" s="20">
+        <f>$D$100*((100-C95)/100)</f>
+        <v>2743.92</v>
+      </c>
+      <c r="E95" s="20">
+        <f>D95/$D$99</f>
+        <v>1850</v>
+      </c>
+      <c r="F95" s="20">
+        <f>$D$100*(C95/100)</f>
+        <v>222.48</v>
+      </c>
+      <c r="G95" s="68"/>
+      <c r="H95" s="68"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="59"/>
+      <c r="B96" s="53"/>
+      <c r="C96" s="30">
+        <v>11.25</v>
+      </c>
+      <c r="D96" s="38">
+        <f>$D$100*((100-C96)/100)</f>
+        <v>2632.68</v>
+      </c>
+      <c r="E96" s="20">
+        <f>D96/$D$99</f>
+        <v>1774.9999999999998</v>
+      </c>
+      <c r="F96" s="38">
+        <f>$D$100*(C96/100)</f>
+        <v>333.72</v>
+      </c>
+      <c r="G96" s="71"/>
+      <c r="H96" s="68"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="59"/>
+      <c r="B97" s="53"/>
+      <c r="C97" s="15">
+        <v>15</v>
+      </c>
+      <c r="D97" s="20">
+        <f>$D$100*((100-C97)/100)</f>
+        <v>2521.44</v>
+      </c>
+      <c r="E97" s="20">
+        <f>D97/$D$99</f>
+        <v>1700</v>
+      </c>
+      <c r="F97" s="20">
+        <f>$D$100*(C97/100)</f>
+        <v>444.96</v>
+      </c>
+      <c r="G97" s="71"/>
+      <c r="H97" s="68"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="59"/>
+      <c r="B98" s="53"/>
+      <c r="G98" s="69"/>
+      <c r="H98" s="69"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="59"/>
+      <c r="B99" s="53"/>
+      <c r="C99" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D99" s="45">
+        <v>1.4832000000000001</v>
+      </c>
+      <c r="E99" s="45"/>
+      <c r="F99" s="45">
+        <v>1.2</v>
+      </c>
+      <c r="G99" s="72"/>
+      <c r="H99" s="73"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="59"/>
+      <c r="B100" s="53"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="16">
+        <f>C1*D99</f>
         <v>2966.4</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="E100" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F95" s="16"/>
-      <c r="G95" s="73"/>
-      <c r="H95" s="73"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="64"/>
-      <c r="B96" s="64"/>
-      <c r="C96" s="16"/>
-      <c r="D96" s="16"/>
-      <c r="E96" s="16"/>
-      <c r="F96" s="16"/>
-      <c r="G96" s="73"/>
-      <c r="H96" s="73"/>
-      <c r="J96" s="5" t="s">
+      <c r="F100" s="16"/>
+      <c r="G100" s="73"/>
+      <c r="H100" s="73"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="64"/>
+      <c r="B101" s="64"/>
+      <c r="C101" s="16"/>
+      <c r="D101" s="16"/>
+      <c r="E101" s="16"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="73"/>
+      <c r="H101" s="73"/>
+      <c r="J101" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="K96" s="5" t="s">
+      <c r="K101" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="L96" s="5" t="s">
+      <c r="L101" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A97" s="62" t="s">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="B97" s="54">
+      <c r="B102" s="54">
         <v>0</v>
       </c>
-      <c r="C97" s="52">
-        <f>(F97/(D97+F97))*100</f>
+      <c r="C102" s="52">
+        <f>(F102/(D102+F102))*100</f>
         <v>0.24548542220129804</v>
       </c>
-      <c r="D97" s="6">
-        <f>$D$94*E97</f>
+      <c r="D102" s="6">
+        <f>$D$99*E102</f>
         <v>2966.4</v>
       </c>
-      <c r="E97" s="6">
+      <c r="E102" s="6">
         <v>2000</v>
       </c>
-      <c r="F97" s="6">
+      <c r="F102" s="6">
         <v>7.3</v>
       </c>
-      <c r="G97" s="74"/>
-      <c r="H97" s="73"/>
-      <c r="L97" s="58">
+      <c r="G102" s="74"/>
+      <c r="H102" s="73"/>
+      <c r="L102" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" s="62"/>
-      <c r="B98" s="54">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="62"/>
+      <c r="B103" s="54">
         <v>1</v>
       </c>
-      <c r="C98" s="52">
-        <f t="shared" ref="C98" si="28">(F98/(D98+F98))*100</f>
+      <c r="C103" s="52">
+        <f t="shared" ref="C103" si="28">(F103/(D103+F103))*100</f>
         <v>7.5875055383252095</v>
       </c>
-      <c r="D98" s="6">
-        <f>$D$94*E98</f>
+      <c r="D103" s="6">
+        <f>$D$99*E103</f>
         <v>2669.76</v>
       </c>
-      <c r="E98" s="6">
+      <c r="E103" s="6">
         <v>1800</v>
       </c>
-      <c r="F98" s="6">
+      <c r="F103" s="6">
         <v>219.2</v>
       </c>
-      <c r="G98" s="71" t="s">
+      <c r="G103" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="H98" s="73"/>
-      <c r="L98" s="58">
+      <c r="H103" s="73"/>
+      <c r="L103" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G99" s="69"/>
-      <c r="H99" s="69"/>
-      <c r="L99" s="58"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" s="59" t="s">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G104" s="69"/>
+      <c r="H104" s="69"/>
+      <c r="L104" s="58"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="B100" s="53"/>
-      <c r="C100" s="31" t="s">
+      <c r="B105" s="53"/>
+      <c r="C105" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D105" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E100" s="5" t="s">
+      <c r="E105" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F100" s="5" t="s">
+      <c r="F105" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G100" s="70"/>
-      <c r="H100" s="69"/>
-      <c r="L100" s="58"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A101" s="59"/>
-      <c r="B101" s="53"/>
-      <c r="C101" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D101" s="20">
-        <f>$D$108*((100-C101)/100)</f>
-        <v>2644.3724999999999</v>
-      </c>
-      <c r="E101" s="20">
-        <f>D101/$D$107</f>
-        <v>1995</v>
-      </c>
-      <c r="F101" s="20">
-        <f>$D$108*(C101/100)</f>
-        <v>6.6275000000000004</v>
-      </c>
-      <c r="G101" s="68"/>
-      <c r="H101" s="68"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A102" s="59"/>
-      <c r="B102" s="53"/>
-      <c r="C102" s="30">
-        <v>3.75</v>
-      </c>
-      <c r="D102" s="38">
-        <f t="shared" ref="D102:D105" si="29">$D$108*((100-C102)/100)</f>
-        <v>2551.5875000000001</v>
-      </c>
-      <c r="E102" s="20">
-        <f t="shared" ref="E102:E105" si="30">D102/$D$107</f>
-        <v>1925.0000000000002</v>
-      </c>
-      <c r="F102" s="38">
-        <f t="shared" ref="F102:F105" si="31">$D$108*(C102/100)</f>
-        <v>99.412499999999994</v>
-      </c>
-      <c r="G102" s="68"/>
-      <c r="H102" s="68"/>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A103" s="59"/>
-      <c r="B103" s="53"/>
-      <c r="C103" s="15">
-        <v>7.5</v>
-      </c>
-      <c r="D103" s="20">
-        <f t="shared" si="29"/>
-        <v>2452.1750000000002</v>
-      </c>
-      <c r="E103" s="20">
-        <f t="shared" si="30"/>
-        <v>1850.0000000000002</v>
-      </c>
-      <c r="F103" s="20">
-        <f t="shared" si="31"/>
-        <v>198.82499999999999</v>
-      </c>
-      <c r="G103" s="68"/>
-      <c r="H103" s="68"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A104" s="59"/>
-      <c r="B104" s="53"/>
-      <c r="C104" s="30">
-        <v>11.25</v>
-      </c>
-      <c r="D104" s="38">
-        <f t="shared" si="29"/>
-        <v>2352.7624999999998</v>
-      </c>
-      <c r="E104" s="20">
-        <f t="shared" si="30"/>
-        <v>1775</v>
-      </c>
-      <c r="F104" s="38">
-        <f t="shared" si="31"/>
-        <v>298.23750000000001</v>
-      </c>
-      <c r="G104" s="71"/>
-      <c r="H104" s="68"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A105" s="59"/>
-      <c r="B105" s="53"/>
-      <c r="C105" s="15">
-        <v>15</v>
-      </c>
-      <c r="D105" s="20">
-        <f t="shared" si="29"/>
-        <v>2253.35</v>
-      </c>
-      <c r="E105" s="20">
-        <f t="shared" si="30"/>
-        <v>1700</v>
-      </c>
-      <c r="F105" s="20">
-        <f t="shared" si="31"/>
-        <v>397.65</v>
-      </c>
-      <c r="G105" s="71"/>
-      <c r="H105" s="68"/>
+      <c r="G105" s="70"/>
+      <c r="H105" s="69"/>
+      <c r="L105" s="58"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="59"/>
       <c r="B106" s="53"/>
-      <c r="G106" s="69"/>
-      <c r="H106" s="69"/>
+      <c r="C106" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="D106" s="20">
+        <f>$D$113*((100-C106)/100)</f>
+        <v>2644.3724999999999</v>
+      </c>
+      <c r="E106" s="20">
+        <f>D106/$D$112</f>
+        <v>1995</v>
+      </c>
+      <c r="F106" s="20">
+        <f>$D$113*(C106/100)</f>
+        <v>6.6275000000000004</v>
+      </c>
+      <c r="G106" s="68"/>
+      <c r="H106" s="68"/>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="59"/>
       <c r="B107" s="53"/>
-      <c r="C107" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D107" s="45">
-        <v>1.3254999999999999</v>
-      </c>
-      <c r="E107" s="45"/>
-      <c r="F107" s="45">
-        <v>1.2</v>
-      </c>
-      <c r="G107" s="72"/>
-      <c r="H107" s="73"/>
+      <c r="C107" s="30">
+        <v>3.75</v>
+      </c>
+      <c r="D107" s="38">
+        <f t="shared" ref="D107:D110" si="29">$D$113*((100-C107)/100)</f>
+        <v>2551.5875000000001</v>
+      </c>
+      <c r="E107" s="20">
+        <f t="shared" ref="E107:E110" si="30">D107/$D$112</f>
+        <v>1925.0000000000002</v>
+      </c>
+      <c r="F107" s="38">
+        <f t="shared" ref="F107:F110" si="31">$D$113*(C107/100)</f>
+        <v>99.412499999999994</v>
+      </c>
+      <c r="G107" s="68"/>
+      <c r="H107" s="68"/>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="59"/>
       <c r="B108" s="53"/>
-      <c r="C108" s="16"/>
-      <c r="D108" s="16">
-        <f>C1*D107</f>
+      <c r="C108" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="D108" s="20">
+        <f t="shared" si="29"/>
+        <v>2452.1750000000002</v>
+      </c>
+      <c r="E108" s="20">
+        <f t="shared" si="30"/>
+        <v>1850.0000000000002</v>
+      </c>
+      <c r="F108" s="20">
+        <f t="shared" si="31"/>
+        <v>198.82499999999999</v>
+      </c>
+      <c r="G108" s="68"/>
+      <c r="H108" s="68"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A109" s="59"/>
+      <c r="B109" s="53"/>
+      <c r="C109" s="30">
+        <v>11.25</v>
+      </c>
+      <c r="D109" s="38">
+        <f t="shared" si="29"/>
+        <v>2352.7624999999998</v>
+      </c>
+      <c r="E109" s="20">
+        <f t="shared" si="30"/>
+        <v>1775</v>
+      </c>
+      <c r="F109" s="38">
+        <f t="shared" si="31"/>
+        <v>298.23750000000001</v>
+      </c>
+      <c r="G109" s="71"/>
+      <c r="H109" s="68"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A110" s="59"/>
+      <c r="B110" s="53"/>
+      <c r="C110" s="15">
+        <v>15</v>
+      </c>
+      <c r="D110" s="20">
+        <f t="shared" si="29"/>
+        <v>2253.35</v>
+      </c>
+      <c r="E110" s="20">
+        <f t="shared" si="30"/>
+        <v>1700</v>
+      </c>
+      <c r="F110" s="20">
+        <f t="shared" si="31"/>
+        <v>397.65</v>
+      </c>
+      <c r="G110" s="71"/>
+      <c r="H110" s="68"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111" s="59"/>
+      <c r="B111" s="53"/>
+      <c r="G111" s="69"/>
+      <c r="H111" s="69"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A112" s="59"/>
+      <c r="B112" s="53"/>
+      <c r="C112" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D112" s="45">
+        <v>1.3254999999999999</v>
+      </c>
+      <c r="E112" s="45"/>
+      <c r="F112" s="45">
+        <v>1.2</v>
+      </c>
+      <c r="G112" s="72"/>
+      <c r="H112" s="73"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" s="59"/>
+      <c r="B113" s="53"/>
+      <c r="C113" s="16"/>
+      <c r="D113" s="16">
+        <f>C1*D112</f>
         <v>2651</v>
       </c>
-      <c r="E108" s="16" t="s">
+      <c r="E113" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F108" s="16"/>
-      <c r="G108" s="73"/>
-      <c r="H108" s="73"/>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G109" s="69"/>
-      <c r="H109" s="69"/>
-      <c r="J109" s="5" t="s">
+      <c r="F113" s="16"/>
+      <c r="G113" s="73"/>
+      <c r="H113" s="73"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G114" s="69"/>
+      <c r="H114" s="69"/>
+      <c r="J114" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="K109" s="5" t="s">
+      <c r="K114" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="L109" s="5" t="s">
+      <c r="L114" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A110" s="60" t="s">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="B110" s="56">
+      <c r="B115" s="56">
         <v>3</v>
       </c>
-      <c r="C110" s="20">
-        <f>(F110/(D110+F110))*100</f>
+      <c r="C115" s="20">
+        <f>(F115/(D115+F115))*100</f>
         <v>0.29336542801263726</v>
       </c>
-      <c r="D110" s="4">
-        <f>$D$107*E110</f>
+      <c r="D115" s="4">
+        <f>$D$112*E115</f>
         <v>2651</v>
       </c>
-      <c r="E110" s="4">
+      <c r="E115" s="4">
         <v>2000</v>
       </c>
-      <c r="F110" s="4">
+      <c r="F115" s="4">
         <v>7.8</v>
       </c>
-      <c r="G110" s="74"/>
-      <c r="H110" s="69"/>
-      <c r="L110" s="58">
+      <c r="G115" s="74"/>
+      <c r="H115" s="69"/>
+      <c r="L115" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A111" s="60"/>
-      <c r="B111" s="56">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" s="60"/>
+      <c r="B116" s="56">
         <v>4</v>
       </c>
-      <c r="C111" s="20">
-        <f t="shared" ref="C111" si="32">(F111/(D111+F111))*100</f>
+      <c r="C116" s="20">
+        <f t="shared" ref="C116" si="32">(F116/(D116+F116))*100</f>
         <v>7.6056228943190192</v>
       </c>
-      <c r="D111" s="4">
-        <f>$D$107*E111</f>
+      <c r="D116" s="4">
+        <f>$D$112*E116</f>
         <v>2385.8999999999996</v>
       </c>
-      <c r="E111" s="4">
+      <c r="E116" s="4">
         <v>1800</v>
       </c>
-      <c r="F111" s="4">
+      <c r="F116" s="4">
         <v>196.4</v>
       </c>
-      <c r="G111" s="71" t="s">
+      <c r="G116" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="H111" s="69"/>
-      <c r="L111" s="58">
+      <c r="H116" s="69"/>
+      <c r="L116" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G112" s="69"/>
-      <c r="H112" s="69"/>
-      <c r="L112" s="58"/>
-    </row>
-    <row r="113" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="59" t="s">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G117" s="69"/>
+      <c r="H117" s="69"/>
+      <c r="L117" s="58"/>
+    </row>
+    <row r="118" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="B113" s="53"/>
-      <c r="C113" s="31" t="s">
+      <c r="B118" s="53"/>
+      <c r="C118" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="D118" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E113" s="5" t="s">
+      <c r="E118" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F113" s="5" t="s">
+      <c r="F118" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I113" s="36"/>
-      <c r="L113" s="58"/>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="59"/>
-      <c r="B114" s="53"/>
-      <c r="C114" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D114" s="20">
-        <f>$D$121*((100-C114)/100)</f>
-        <v>1895.25</v>
-      </c>
-      <c r="E114" s="20">
-        <f>D114/$D$120</f>
-        <v>1995</v>
-      </c>
-      <c r="F114" s="20">
-        <f>$D$121*(C114/100)</f>
-        <v>4.75</v>
-      </c>
-      <c r="G114" s="20"/>
-      <c r="H114" s="20"/>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A115" s="59"/>
-      <c r="B115" s="53"/>
-      <c r="C115" s="15">
-        <v>3.75</v>
-      </c>
-      <c r="D115" s="20">
-        <f t="shared" ref="D115:D118" si="33">$D$121*((100-C115)/100)</f>
-        <v>1828.75</v>
-      </c>
-      <c r="E115" s="20">
-        <f t="shared" ref="E115:E118" si="34">D115/$D$120</f>
-        <v>1925</v>
-      </c>
-      <c r="F115" s="20">
-        <f t="shared" ref="F115:F118" si="35">$D$121*(C115/100)</f>
-        <v>71.25</v>
-      </c>
-      <c r="G115" s="20"/>
-      <c r="H115" s="20"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116" s="59"/>
-      <c r="B116" s="53"/>
-      <c r="C116" s="15">
-        <v>7.5</v>
-      </c>
-      <c r="D116" s="20">
-        <f t="shared" si="33"/>
-        <v>1757.5</v>
-      </c>
-      <c r="E116" s="20">
-        <f t="shared" si="34"/>
-        <v>1850</v>
-      </c>
-      <c r="F116" s="20">
-        <f t="shared" si="35"/>
-        <v>142.5</v>
-      </c>
-      <c r="G116" s="20"/>
-      <c r="H116" s="20"/>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" s="59"/>
-      <c r="B117" s="53"/>
-      <c r="C117" s="15">
-        <v>11.25</v>
-      </c>
-      <c r="D117" s="20">
-        <f t="shared" si="33"/>
-        <v>1686.25</v>
-      </c>
-      <c r="E117" s="20">
-        <f t="shared" si="34"/>
-        <v>1775</v>
-      </c>
-      <c r="F117" s="20">
-        <f t="shared" si="35"/>
-        <v>213.75</v>
-      </c>
-      <c r="G117" s="20"/>
-      <c r="H117" s="20"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A118" s="59"/>
-      <c r="B118" s="53"/>
-      <c r="C118" s="15">
-        <v>15</v>
-      </c>
-      <c r="D118" s="20">
-        <f t="shared" si="33"/>
-        <v>1615</v>
-      </c>
-      <c r="E118" s="20">
-        <f t="shared" si="34"/>
-        <v>1700</v>
-      </c>
-      <c r="F118" s="20">
-        <f t="shared" si="35"/>
-        <v>285</v>
-      </c>
-      <c r="G118" s="20"/>
-      <c r="H118" s="20"/>
+      <c r="I118" s="36"/>
+      <c r="L118" s="58"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="59"/>
       <c r="B119" s="53"/>
+      <c r="C119" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="D119" s="20">
+        <f>$D$126*((100-C119)/100)</f>
+        <v>1895.25</v>
+      </c>
+      <c r="E119" s="20">
+        <f>D119/$D$125</f>
+        <v>1995</v>
+      </c>
+      <c r="F119" s="20">
+        <f>$D$126*(C119/100)</f>
+        <v>4.75</v>
+      </c>
+      <c r="G119" s="20"/>
+      <c r="H119" s="20"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="59"/>
       <c r="B120" s="53"/>
-      <c r="C120" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D120" s="45">
-        <v>0.95</v>
-      </c>
-      <c r="E120" s="45"/>
-      <c r="F120" s="45">
-        <v>1.07</v>
-      </c>
-      <c r="G120" s="45"/>
-      <c r="H120" s="16"/>
+      <c r="C120" s="15">
+        <v>3.75</v>
+      </c>
+      <c r="D120" s="20">
+        <f t="shared" ref="D120:D123" si="33">$D$126*((100-C120)/100)</f>
+        <v>1828.75</v>
+      </c>
+      <c r="E120" s="20">
+        <f t="shared" ref="E120:E123" si="34">D120/$D$125</f>
+        <v>1925</v>
+      </c>
+      <c r="F120" s="20">
+        <f t="shared" ref="F120:F123" si="35">$D$126*(C120/100)</f>
+        <v>71.25</v>
+      </c>
+      <c r="G120" s="20"/>
+      <c r="H120" s="20"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="59"/>
       <c r="B121" s="53"/>
-      <c r="C121" s="16"/>
-      <c r="D121" s="16">
-        <f>C1*D120</f>
+      <c r="C121" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="D121" s="20">
+        <f t="shared" si="33"/>
+        <v>1757.5</v>
+      </c>
+      <c r="E121" s="20">
+        <f t="shared" si="34"/>
+        <v>1850</v>
+      </c>
+      <c r="F121" s="20">
+        <f t="shared" si="35"/>
+        <v>142.5</v>
+      </c>
+      <c r="G121" s="20"/>
+      <c r="H121" s="20"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A122" s="59"/>
+      <c r="B122" s="53"/>
+      <c r="C122" s="15">
+        <v>11.25</v>
+      </c>
+      <c r="D122" s="20">
+        <f t="shared" si="33"/>
+        <v>1686.25</v>
+      </c>
+      <c r="E122" s="20">
+        <f t="shared" si="34"/>
+        <v>1775</v>
+      </c>
+      <c r="F122" s="20">
+        <f t="shared" si="35"/>
+        <v>213.75</v>
+      </c>
+      <c r="G122" s="20"/>
+      <c r="H122" s="20"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123" s="59"/>
+      <c r="B123" s="53"/>
+      <c r="C123" s="15">
+        <v>15</v>
+      </c>
+      <c r="D123" s="20">
+        <f t="shared" si="33"/>
+        <v>1615</v>
+      </c>
+      <c r="E123" s="20">
+        <f t="shared" si="34"/>
+        <v>1700</v>
+      </c>
+      <c r="F123" s="20">
+        <f t="shared" si="35"/>
+        <v>285</v>
+      </c>
+      <c r="G123" s="20"/>
+      <c r="H123" s="20"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" s="59"/>
+      <c r="B124" s="53"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" s="59"/>
+      <c r="B125" s="53"/>
+      <c r="C125" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D125" s="45">
+        <v>0.95</v>
+      </c>
+      <c r="E125" s="45"/>
+      <c r="F125" s="45">
+        <v>1.07</v>
+      </c>
+      <c r="G125" s="45"/>
+      <c r="H125" s="16"/>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126" s="59"/>
+      <c r="B126" s="53"/>
+      <c r="C126" s="16"/>
+      <c r="D126" s="16">
+        <f>C1*D125</f>
         <v>1900</v>
       </c>
-      <c r="E121" s="16" t="s">
+      <c r="E126" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F121" s="16"/>
-      <c r="G121" s="16"/>
-      <c r="H121" s="16"/>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J122" s="5" t="s">
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
+      <c r="H126" s="16"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J127" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="K122" s="5" t="s">
+      <c r="K127" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="L122" s="5" t="s">
+      <c r="L127" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A123" s="65" t="s">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="B123" s="54">
+      <c r="B128" s="54">
         <v>6</v>
       </c>
-      <c r="C123" s="51">
-        <f>(F123/(D123+F123))*100</f>
+      <c r="C128" s="51">
+        <f>(F128/(D128+F128))*100</f>
         <v>0.61202071454726159</v>
       </c>
-      <c r="D123" s="41">
-        <f>$D$120*E123</f>
+      <c r="D128" s="41">
+        <f>$D$125*E128</f>
         <v>1900</v>
       </c>
-      <c r="E123" s="41">
+      <c r="E128" s="41">
         <v>2000</v>
       </c>
-      <c r="F123" s="41">
+      <c r="F128" s="41">
         <v>11.7</v>
       </c>
-      <c r="G123" s="74" t="s">
+      <c r="G128" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="L123" s="58">
+      <c r="L128" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A124" s="65"/>
-      <c r="B124" s="54">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" s="65"/>
+      <c r="B129" s="54">
         <v>7</v>
       </c>
-      <c r="C124" s="51">
-        <f t="shared" ref="C124:C127" si="36">(F124/(D124+F124))*100</f>
+      <c r="C129" s="51">
+        <f t="shared" ref="C129:C132" si="36">(F129/(D129+F129))*100</f>
         <v>4.9399620813145146</v>
       </c>
-      <c r="D124" s="41">
-        <f>$D$120*E124</f>
+      <c r="D129" s="41">
+        <f>$D$125*E129</f>
         <v>1805</v>
       </c>
-      <c r="E124" s="41">
+      <c r="E129" s="41">
         <v>1900</v>
       </c>
-      <c r="F124" s="41">
+      <c r="F129" s="41">
         <v>93.8</v>
       </c>
-      <c r="G124" s="74" t="s">
+      <c r="G129" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="L124" s="58">
+      <c r="L129" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125" s="65"/>
-      <c r="B125" s="54">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A130" s="65"/>
+      <c r="B130" s="54">
         <v>8</v>
       </c>
-      <c r="C125" s="51">
+      <c r="C130" s="51">
         <f t="shared" si="36"/>
         <v>8.0002152041749603</v>
       </c>
-      <c r="D125" s="41">
-        <f>$D$120*E125</f>
+      <c r="D130" s="41">
+        <f>$D$125*E130</f>
         <v>1710</v>
       </c>
-      <c r="E125" s="41">
+      <c r="E130" s="41">
         <v>1800</v>
       </c>
-      <c r="F125" s="41">
+      <c r="F130" s="41">
         <v>148.69999999999999</v>
       </c>
-      <c r="G125" s="74" t="s">
+      <c r="G130" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="L125" s="58">
+      <c r="L130" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A126" s="65"/>
-      <c r="B126" s="54">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A131" s="65"/>
+      <c r="B131" s="54">
         <v>9</v>
       </c>
-      <c r="C126" s="51">
+      <c r="C131" s="51">
         <f t="shared" si="36"/>
         <v>11.43108717045631</v>
       </c>
-      <c r="D126" s="41">
-        <f>$D$120*E126</f>
+      <c r="D131" s="41">
+        <f>$D$125*E131</f>
         <v>1710</v>
       </c>
-      <c r="E126" s="41">
+      <c r="E131" s="41">
         <v>1800</v>
       </c>
-      <c r="F126" s="41">
+      <c r="F131" s="41">
         <v>220.7</v>
       </c>
-      <c r="G126" s="74" t="s">
+      <c r="G131" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="L126" s="58">
+      <c r="L131" s="58">
         <v>20</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A127" s="65"/>
-      <c r="B127" s="54">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A132" s="65"/>
+      <c r="B132" s="54">
         <v>10</v>
       </c>
-      <c r="C127" s="51">
+      <c r="C132" s="51">
         <f t="shared" si="36"/>
         <v>15.165204601565371</v>
       </c>
-      <c r="D127" s="41">
-        <f>$D$120*E127</f>
+      <c r="D132" s="41">
+        <f>$D$125*E132</f>
         <v>1615</v>
       </c>
-      <c r="E127" s="41">
+      <c r="E132" s="41">
         <v>1700</v>
       </c>
-      <c r="F127" s="41">
+      <c r="F132" s="41">
         <v>288.7</v>
       </c>
-      <c r="G127" s="74" t="s">
+      <c r="G132" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="L127" s="58">
+      <c r="L132" s="58">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A123:A127"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A56:A64"/>
-    <mergeCell ref="A77:A85"/>
-    <mergeCell ref="A87:A95"/>
-    <mergeCell ref="A100:A108"/>
-    <mergeCell ref="A113:A121"/>
-    <mergeCell ref="A71:A75"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="A128:A132"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="A82:A90"/>
+    <mergeCell ref="A92:A100"/>
+    <mergeCell ref="A105:A113"/>
+    <mergeCell ref="A118:A126"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A115:A116"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="A13:A21"/>
-    <mergeCell ref="A35:A43"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A36:A44"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A53:A57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>